<commit_message>
Added popups, indentation fix, comments
</commit_message>
<xml_diff>
--- a/test_data/test.xlsx
+++ b/test_data/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>OR</t>
+  </si>
+  <si>
+    <t>Brittany</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>1406 SE Stark St.</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,6 +541,26 @@
         <v>97214</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>97214</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Moved around TODOs, added a couple options for findAddressFields
</commit_message>
<xml_diff>
--- a/test_data/test.xlsx
+++ b/test_data/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>First Name</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -497,9 +497,6 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2">
-        <v>97405</v>
-      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
@@ -530,9 +527,6 @@
       </c>
       <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>

</xml_diff>